<commit_message>
Final changes, code used for thesis submission
</commit_message>
<xml_diff>
--- a/section_configuration.xlsx
+++ b/section_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antig\PycharmProjects\sectionanalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32796C63-0544-4452-A3D2-0566E2944FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314F58DC-6088-4ACD-842A-EE940AD98E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71AF6A26-CBEA-44DB-BF41-AF44417DE945}"/>
+    <workbookView xWindow="3510" yWindow="720" windowWidth="19845" windowHeight="15480" xr2:uid="{71AF6A26-CBEA-44DB-BF41-AF44417DE945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,6 +216,7 @@
       <sheetName val="600x600"/>
       <sheetName val="600x600 (2)"/>
       <sheetName val="Sheet4"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -764,6 +765,7 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1069,7 +1071,7 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>